<commit_message>
Added new automapper pipeline by adding reranking classes using LLM
</commit_message>
<xml_diff>
--- a/data/excel_files/Abbreviation.xlsx
+++ b/data/excel_files/Abbreviation.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sufarhansudaryo/Documents/Work/semantic-automapper/data/excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64192268-7BB6-5741-8F5E-88F99442A7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16EE3B04-33EA-EF47-8E77-55D14057C35C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19780" xr2:uid="{6CDC6E38-5C14-974E-BA44-9137CC382015}"/>
+    <workbookView xWindow="2260" yWindow="22360" windowWidth="34200" windowHeight="21380" xr2:uid="{6CDC6E38-5C14-974E-BA44-9137CC382015}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="48">
   <si>
     <t>Bolt Matrix</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Mine Hangers</t>
   </si>
   <si>
-    <t xml:space="preserve">AH = High Strength Steel, AS = Standard Strength Steel,  AX = Extra High Strength, Steel AT = HSA840 Steel, ATR = AT steel with High Rib, AXR = AX steel with High Rib </t>
-  </si>
-  <si>
     <t>DS = Double ended bolt Standard Strength, CS = Solid Deformed Bar, DCS = Double Corrosion Protection Steel bell</t>
   </si>
   <si>
@@ -144,6 +141,45 @@
   </si>
   <si>
     <t xml:space="preserve">B = Bolt without continuous thread, D =  Dowel with continuous thread, DH = Dowel Hollow </t>
+  </si>
+  <si>
+    <t>G = Galvanised, TD = Thermal Diffused, TS = Thermal Metal Spray, P = Plas coating</t>
+  </si>
+  <si>
+    <t>WA =  Perth, B = Brisbane, no suffix = Newcastle</t>
+  </si>
+  <si>
+    <t>G = Galvanised, DB = Debonding Tube, GT = Grout Tube, BT =Breather Tube, RD = Refer Drawing, Q =Steel Aglet</t>
+  </si>
+  <si>
+    <t>WA = Freight Cost, B = Brisbane, N = Sea freight</t>
+  </si>
+  <si>
+    <t>WA = Freight included to Perth, B=Brisbane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G = Galvanised, TD = Thermal Diffused, TS = Thermal Metal Spray, P = Plas coating, R = Rumbled, XB = Bundled for Galvanisining </t>
+  </si>
+  <si>
+    <t>FL = Flared hole, N = Indicator Posts, SS316= Stainless Steel</t>
+  </si>
+  <si>
+    <t>B=Brisbane, WA = Western Australia, EXP=Export</t>
+  </si>
+  <si>
+    <t>WA = Western Australia, B = Brisbane</t>
+  </si>
+  <si>
+    <t>WA = Western Australia, B = Brisbane, E=Export, HP = Half Pallet, R = Exworks Rocbolt, D=Dunnage bags</t>
+  </si>
+  <si>
+    <t>G = Galvanised, EZ = Electroplated Zinc</t>
+  </si>
+  <si>
+    <t>7948 = Closed loop in 12mm round bar to suit 20mm Thread Bar (36AF Nut), 7985 = Closed Loop 12mm Round Bar to suit M24 thread (OZ nut 36AF), 8033 = 3 x Open Hooks in 16mm round bar to suit 110mm pipe, 8036 = 4 x Open Hooks in 16mm round bar to suit 110mm pipe, 7471 = Single keyhole bracket with 26mm mounting hole, 7513 = Fan hanger "T" shaped in 16 &amp; 12mm plate with a single keyhole, 7514 = 6 x Keyholes with 3 x 28mm mounting holes, 7523 = 3 Keyholes and 8mm chains with 3 x 26mm mounting holes, 7525 = 1 Keyhole and 8mm chain with 1 x 26mm mounting hole, 7526 = 7 Keyholes with 3 x 26mm mounting holes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AH = High Strength Steel, AS = Standard Strength Steel,  AX = Extra High Strength Steel, AT = HSA840 Steel, ATR = AT steel with High Rib, AXR = AX steel with High Rib </t>
   </si>
 </sst>
 </file>
@@ -515,21 +551,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E46EB0-B57B-844B-B4D5-057496B7A302}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="252.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="255.6640625" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -537,7 +573,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -545,7 +581,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -553,7 +589,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -561,23 +597,23 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -585,146 +621,239 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+      <c r="B32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>19</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B35" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>